<commit_message>
change name of method, added new grafana json-file
</commit_message>
<xml_diff>
--- a/Last_Updated.xlsx
+++ b/Last_Updated.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1150"/>
+  <dimension ref="A1:B1156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11931,9 +11931,69 @@
     </row>
     <row r="1150">
       <c r="A1150" s="2" t="n">
-        <v>44272.92305555556</v>
+        <v>44272.92305555557</v>
       </c>
       <c r="B1150" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" s="2" t="n">
+        <v>44273.69190972222</v>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" s="2" t="n">
+        <v>44273.69310185185</v>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" s="2" t="n">
+        <v>44273.70390046296</v>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" s="2" t="n">
+        <v>44273.70487268519</v>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" s="2" t="n">
+        <v>44273.72856481482</v>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" s="2" t="n">
+        <v>44273.72936342593</v>
+      </c>
+      <c r="B1156" t="inlineStr">
         <is>
           <t>finished</t>
         </is>

</xml_diff>

<commit_message>
added print for debug purpose on heroku
</commit_message>
<xml_diff>
--- a/Last_Updated.xlsx
+++ b/Last_Updated.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2484"/>
+  <dimension ref="A1:B2486"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25279,6 +25279,26 @@
         </is>
       </c>
     </row>
+    <row r="2485">
+      <c r="A2485" s="2" t="n">
+        <v>44563.88137731481</v>
+      </c>
+      <c r="B2485" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="2486">
+      <c r="A2486" s="2" t="n">
+        <v>44563.88932870371</v>
+      </c>
+      <c r="B2486" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changed from .xlsx to csv. csv is around 2x larger, but much faster to read into dataframe.
</commit_message>
<xml_diff>
--- a/Last_Updated.xlsx
+++ b/Last_Updated.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2489"/>
+  <dimension ref="A1:B2507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25329,6 +25329,186 @@
         </is>
       </c>
     </row>
+    <row r="2490">
+      <c r="A2490" s="2" t="n">
+        <v>44563.92744212963</v>
+      </c>
+      <c r="B2490" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2491">
+      <c r="A2491" s="2" t="n">
+        <v>44563.93055555555</v>
+      </c>
+      <c r="B2491" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2492">
+      <c r="A2492" s="2" t="n">
+        <v>44563.93125</v>
+      </c>
+      <c r="B2492" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2493">
+      <c r="A2493" s="2" t="n">
+        <v>44563.93253472223</v>
+      </c>
+      <c r="B2493" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="2494">
+      <c r="A2494" s="2" t="n">
+        <v>44564.20869212963</v>
+      </c>
+      <c r="B2494" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2495">
+      <c r="A2495" s="2" t="n">
+        <v>44564.58358796296</v>
+      </c>
+      <c r="B2495" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2496">
+      <c r="A2496" s="2" t="n">
+        <v>44564.58488425926</v>
+      </c>
+      <c r="B2496" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="2497">
+      <c r="A2497" s="2" t="n">
+        <v>44564.79607638889</v>
+      </c>
+      <c r="B2497" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2498">
+      <c r="A2498" s="2" t="n">
+        <v>44564.79733796296</v>
+      </c>
+      <c r="B2498" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
+    <row r="2499">
+      <c r="A2499" s="2" t="n">
+        <v>44564.82525462963</v>
+      </c>
+      <c r="B2499" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2500">
+      <c r="A2500" s="2" t="n">
+        <v>44564.83916666666</v>
+      </c>
+      <c r="B2500" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2501">
+      <c r="A2501" s="2" t="n">
+        <v>44564.84918981481</v>
+      </c>
+      <c r="B2501" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2502">
+      <c r="A2502" s="2" t="n">
+        <v>44564.85200231482</v>
+      </c>
+      <c r="B2502" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2503">
+      <c r="A2503" s="2" t="n">
+        <v>44564.85327546296</v>
+      </c>
+      <c r="B2503" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2504">
+      <c r="A2504" s="2" t="n">
+        <v>44564.85366898148</v>
+      </c>
+      <c r="B2504" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2505">
+      <c r="A2505" s="2" t="n">
+        <v>44564.85939814815</v>
+      </c>
+      <c r="B2505" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2506">
+      <c r="A2506" s="2" t="n">
+        <v>44564.86420138889</v>
+      </c>
+      <c r="B2506" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2507">
+      <c r="A2507" s="2" t="n">
+        <v>44564.86722222222</v>
+      </c>
+      <c r="B2507" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
log into csv instead ov xlsx some clean up
</commit_message>
<xml_diff>
--- a/Last_Updated.xlsx
+++ b/Last_Updated.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2507"/>
+  <dimension ref="A1:B2509"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25509,6 +25509,26 @@
         </is>
       </c>
     </row>
+    <row r="2508">
+      <c r="A2508" s="2" t="n">
+        <v>44564.87517361111</v>
+      </c>
+      <c r="B2508" t="inlineStr">
+        <is>
+          <t>started</t>
+        </is>
+      </c>
+    </row>
+    <row r="2509">
+      <c r="A2509" s="2" t="n">
+        <v>44564.8758912037</v>
+      </c>
+      <c r="B2509" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>